<commit_message>
Revert "Revert "Merge remote-tracking branch 'origin/master'""
This reverts commit f5359d7b07513c392aa38502f5910fd696fdde4f.
</commit_message>
<xml_diff>
--- a/GitTest01.xlsx
+++ b/GitTest01.xlsx
@@ -19,17 +19,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>아녕하세요</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>첫 변경점</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>두번째 변경점</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -355,42 +351,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C2">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C3">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C4">
-        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>